<commit_message>
Revert to STABLE dropdown (Yes/No) concept
</commit_message>
<xml_diff>
--- a/rhies_OpenMRStoDHIS2Mediator/matchingDico/DHIS2DataElementToOpenMRS.xlsx
+++ b/rhies_OpenMRStoDHIS2Mediator/matchingDico/DHIS2DataElementToOpenMRS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SavicsProject\RHIES\dhis2Projects\DataMapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SavicsProject\RHIES\RHIESMediators\coding\rhies_Mediators\rhies_OpenMRStoDHIS2Mediator\matchingDico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAEF12A-6F9C-4B34-A3BB-3DEAA65F58B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C2E2D4-8FBE-497B-B04D-9D9D45162409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="r45yv7rwDEO" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1007">
   <si>
     <t>DHIS2 dropdown name</t>
   </si>
@@ -3099,16 +3099,10 @@
     <t>DATE_PHARMACY_PICK_UP_HIDE</t>
   </si>
   <si>
-    <t>STABLE HIDE</t>
-  </si>
-  <si>
-    <t>a650f583-8b61-4772-bae0-200dc81a463b</t>
-  </si>
-  <si>
-    <t>TEXT/3cd6f600-26fe-102b-80cb-0017a47871b2</t>
-  </si>
-  <si>
-    <t>TEXT/3cd6f86c-26fe-102b-80cb-0017a47871b2</t>
+    <t>fab9afe9-8c11-4e31-9898-399b083fd9d6</t>
+  </si>
+  <si>
+    <t>STABLE</t>
   </si>
 </sst>
 </file>
@@ -3236,7 +3230,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3306,6 +3300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3394,7 +3394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3481,6 +3481,8 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3793,8 +3795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.921875" defaultRowHeight="14.6"/>
@@ -3811,22 +3813,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
     </row>
     <row r="2" spans="1:9" ht="22.85" customHeight="1">
-      <c r="A2" s="48"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
@@ -4444,22 +4446,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.25" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
     </row>
     <row r="2" spans="1:9" ht="24.55" customHeight="1">
-      <c r="A2" s="48"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
@@ -6093,25 +6095,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="8" customFormat="1" ht="27" customHeight="1">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="53" t="s">
         <v>179</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
       <c r="J1" s="8" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="48"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
@@ -6853,7 +6855,7 @@
       <c r="E36" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="F36" s="53" t="s">
+      <c r="F36" s="55" t="s">
         <v>983</v>
       </c>
       <c r="G36" s="1"/>
@@ -6872,7 +6874,7 @@
       <c r="E37" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="F37" s="54"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -6889,7 +6891,7 @@
       <c r="E38" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F38" s="55"/>
+      <c r="F38" s="57"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -7835,8 +7837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F78C531-5A28-448B-9C94-8E675119435D}">
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="A121" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C152" sqref="C152"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B120" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.921875" defaultRowHeight="14.6"/>
@@ -7853,25 +7855,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>282</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="38.6">
-      <c r="A2" s="48"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
@@ -10049,28 +10051,28 @@
         <v>134</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
-      <c r="A97" s="1">
+    <row r="97" spans="1:9" s="49" customFormat="1">
+      <c r="A97" s="48">
         <v>95</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="48" t="s">
         <v>416</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C97" s="48" t="s">
         <v>415</v>
       </c>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1" t="s">
+      <c r="D97" s="48"/>
+      <c r="E97" s="48"/>
+      <c r="F97" s="48" t="s">
         <v>614</v>
       </c>
-      <c r="G97" s="1" t="s">
+      <c r="G97" s="48" t="s">
         <v>615</v>
       </c>
-      <c r="H97" s="1" t="s">
+      <c r="H97" s="48" t="s">
         <v>556</v>
       </c>
-      <c r="I97" s="1">
+      <c r="I97" s="48">
         <v>134</v>
       </c>
     </row>
@@ -11390,10 +11392,10 @@
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
       <c r="F152" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G152" s="1" t="s">
         <v>1005</v>
-      </c>
-      <c r="G152" s="1" t="s">
-        <v>1006</v>
       </c>
       <c r="H152" s="14" t="s">
         <v>556</v>
@@ -11416,7 +11418,7 @@
         <v>156</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>1007</v>
+        <v>157</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>556</v>
@@ -11439,7 +11441,7 @@
         <v>154</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>1008</v>
+        <v>155</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>556</v>
@@ -12117,11 +12119,11 @@
   <dimension ref="A1:J159"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K8" sqref="K8"/>
       <selection pane="topRight" activeCell="K8" sqref="K8"/>
       <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
-      <selection pane="bottomRight" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomRight" activeCell="F58" sqref="F58:G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="64.61328125" defaultRowHeight="14.6"/>
@@ -12139,25 +12141,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="58" t="s">
         <v>676</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="48"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="3" t="s">
         <v>48</v>
       </c>
@@ -13418,10 +13420,10 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="G58" s="1" t="s">
         <v>1005</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>1006</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>881</v>
@@ -13444,7 +13446,7 @@
         <v>156</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>1007</v>
+        <v>157</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>881</v>
@@ -13467,7 +13469,7 @@
         <v>154</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>1008</v>
+        <v>155</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>881</v>

</xml_diff>

<commit_message>
Edit getDHIS2OverAllTreatmentAdherence function to handle the concept ADHERENCE HIDE
</commit_message>
<xml_diff>
--- a/rhies_OpenMRStoDHIS2Mediator/matchingDico/DHIS2DataElementToOpenMRS.xlsx
+++ b/rhies_OpenMRStoDHIS2Mediator/matchingDico/DHIS2DataElementToOpenMRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SavicsProject\RHIES\RHIESMediators\coding\rhies_Mediators\rhies_OpenMRStoDHIS2Mediator\matchingDico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C2E2D4-8FBE-497B-B04D-9D9D45162409}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F40522-EEA5-46F6-84E3-706B93CD655D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="r45yv7rwDEO" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="1002">
   <si>
     <t>DHIS2 dropdown name</t>
   </si>
@@ -2643,30 +2643,6 @@
     <t>a18bc25f-1757-4568-88a7-d58c4100f7f2</t>
   </si>
   <si>
-    <t>OVERALL TREATMENT ADHERENCE</t>
-  </si>
-  <si>
-    <t>3ce2ad10-26fe-102b-80cb-0017a47871b2</t>
-  </si>
-  <si>
-    <t>POOR</t>
-  </si>
-  <si>
-    <t>3cdef6c0-26fe-102b-80cb-0017a47871b2</t>
-  </si>
-  <si>
-    <t>GOOD</t>
-  </si>
-  <si>
-    <t>3cdef3d2-26fe-102b-80cb-0017a47871b2</t>
-  </si>
-  <si>
-    <t>FAIR</t>
-  </si>
-  <si>
-    <t>3cdef54e-26fe-102b-80cb-0017a47871b2</t>
-  </si>
-  <si>
     <t>CLIENT TPT OUTCOME</t>
   </si>
   <si>
@@ -3103,6 +3079,15 @@
   </si>
   <si>
     <t>STABLE</t>
+  </si>
+  <si>
+    <t>Very Good</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>Text</t>
   </si>
 </sst>
 </file>
@@ -3892,10 +3877,10 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>938</v>
+        <v>930</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>939</v>
+        <v>931</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -3909,16 +3894,16 @@
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="5" t="s">
-        <v>959</v>
+        <v>951</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>968</v>
+        <v>960</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>940</v>
+        <v>932</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>949</v>
+        <v>941</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -3928,16 +3913,16 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="5" t="s">
-        <v>958</v>
+        <v>950</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>971</v>
+        <v>963</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>941</v>
+        <v>933</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>950</v>
+        <v>942</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -3947,16 +3932,16 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="5" t="s">
-        <v>960</v>
+        <v>952</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>976</v>
+        <v>968</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>942</v>
+        <v>934</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>951</v>
+        <v>943</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -3966,16 +3951,16 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="5" t="s">
-        <v>961</v>
+        <v>953</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>974</v>
+        <v>966</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>943</v>
+        <v>935</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>952</v>
+        <v>944</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -3985,16 +3970,16 @@
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="5" t="s">
-        <v>962</v>
+        <v>954</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>975</v>
+        <v>967</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>944</v>
+        <v>936</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>953</v>
+        <v>945</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -4004,16 +3989,16 @@
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="5" t="s">
-        <v>963</v>
+        <v>955</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>973</v>
+        <v>965</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>945</v>
+        <v>937</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>954</v>
+        <v>946</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -4023,16 +4008,16 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="5" t="s">
+        <v>956</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>964</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>972</v>
-      </c>
       <c r="F11" s="5" t="s">
-        <v>946</v>
+        <v>938</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>955</v>
+        <v>947</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -4042,16 +4027,16 @@
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="5" t="s">
-        <v>965</v>
+        <v>957</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>969</v>
+        <v>961</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>947</v>
+        <v>939</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>956</v>
+        <v>948</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -4061,16 +4046,16 @@
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="5" t="s">
-        <v>966</v>
+        <v>958</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>970</v>
+        <v>962</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>948</v>
+        <v>940</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>957</v>
+        <v>949</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -4159,7 +4144,7 @@
         <v>21</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>967</v>
+        <v>959</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>628</v>
@@ -4517,10 +4502,10 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="21" t="s">
-        <v>977</v>
+        <v>969</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>978</v>
+        <v>970</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="39"/>
@@ -4532,7 +4517,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="5" t="s">
-        <v>979</v>
+        <v>971</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>157</v>
@@ -4547,7 +4532,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="5" t="s">
-        <v>980</v>
+        <v>972</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>155</v>
@@ -6856,7 +6841,7 @@
         <v>202</v>
       </c>
       <c r="F36" s="55" t="s">
-        <v>983</v>
+        <v>975</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -6976,10 +6961,10 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="21" t="s">
-        <v>882</v>
+        <v>874</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>883</v>
+        <v>875</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>26</v>
@@ -7068,10 +7053,10 @@
       <c r="D46" s="43"/>
       <c r="E46" s="43"/>
       <c r="F46" s="43" t="s">
-        <v>981</v>
+        <v>973</v>
       </c>
       <c r="G46" s="43" t="s">
-        <v>982</v>
+        <v>974</v>
       </c>
       <c r="H46" s="43" t="s">
         <v>26</v>
@@ -7837,7 +7822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F78C531-5A28-448B-9C94-8E675119435D}">
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B120" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showFormulas="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
@@ -8097,7 +8082,7 @@
         <v>565</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>1002</v>
+        <v>994</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>556</v>
@@ -8274,10 +8259,10 @@
         <v>314</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>985</v>
+        <v>977</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>984</v>
+        <v>976</v>
       </c>
       <c r="H19" s="40" t="s">
         <v>556</v>
@@ -8374,7 +8359,7 @@
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="1" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>578</v>
@@ -8399,10 +8384,10 @@
         <v>325</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="H24" s="14" t="s">
         <v>556</v>
@@ -8424,7 +8409,7 @@
         <v>326</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>579</v>
@@ -8449,7 +8434,7 @@
         <v>327</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>580</v>
@@ -8474,7 +8459,7 @@
         <v>328</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>581</v>
@@ -8499,10 +8484,10 @@
         <v>329</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="H28" s="14" t="s">
         <v>556</v>
@@ -8673,10 +8658,10 @@
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="1" t="s">
-        <v>895</v>
+        <v>887</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>894</v>
+        <v>886</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -8757,7 +8742,7 @@
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="6" t="s">
-        <v>884</v>
+        <v>876</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="1"/>
@@ -9034,7 +9019,7 @@
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="6" t="s">
-        <v>885</v>
+        <v>877</v>
       </c>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -10192,7 +10177,7 @@
         <v>565</v>
       </c>
       <c r="G102" s="41" t="s">
-        <v>1002</v>
+        <v>994</v>
       </c>
       <c r="H102" s="40" t="s">
         <v>556</v>
@@ -11096,10 +11081,10 @@
       <c r="D140" s="40"/>
       <c r="E140" s="40"/>
       <c r="F140" s="40" t="s">
-        <v>986</v>
+        <v>978</v>
       </c>
       <c r="G140" s="40" t="s">
-        <v>987</v>
+        <v>979</v>
       </c>
       <c r="H140" s="40" t="s">
         <v>556</v>
@@ -11392,10 +11377,10 @@
       <c r="D152" s="14"/>
       <c r="E152" s="14"/>
       <c r="F152" s="1" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>1005</v>
+        <v>997</v>
       </c>
       <c r="H152" s="14" t="s">
         <v>556</v>
@@ -12118,12 +12103,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC28AE1-BBA6-488B-8021-D9435874BC68}">
   <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K8" sqref="K8"/>
       <selection pane="topRight" activeCell="K8" sqref="K8"/>
       <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
-      <selection pane="bottomRight" activeCell="F58" sqref="F58:G60"/>
+      <selection pane="bottomRight" activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="64.61328125" defaultRowHeight="14.6"/>
@@ -12200,7 +12185,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I3" s="1">
         <v>135</v>
@@ -12221,7 +12206,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I4" s="1">
         <v>135</v>
@@ -12239,11 +12224,11 @@
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="6" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I5" s="1">
         <v>135</v>
@@ -12262,11 +12247,11 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="6" t="s">
-        <v>992</v>
+        <v>984</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I6" s="1">
         <v>135</v>
@@ -12287,7 +12272,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I7" s="1">
         <v>135</v>
@@ -12311,7 +12296,7 @@
         <v>804</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I8" s="1">
         <v>135</v>
@@ -12332,7 +12317,7 @@
         <v>157</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I9" s="1">
         <v>135</v>
@@ -12355,7 +12340,7 @@
         <v>155</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I10" s="1">
         <v>135</v>
@@ -12375,7 +12360,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I11" s="1">
         <v>135</v>
@@ -12392,7 +12377,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I12" s="1">
         <v>135</v>
@@ -12411,7 +12396,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I13" s="1">
         <v>135</v>
@@ -12435,7 +12420,7 @@
         <v>569</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I14" s="21">
         <v>135</v>
@@ -12452,13 +12437,13 @@
         <v>313</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>989</v>
+        <v>981</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>571</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I15" s="21">
         <v>135</v>
@@ -12477,13 +12462,13 @@
         <v>314</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>985</v>
+        <v>977</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>984</v>
+        <v>976</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I16" s="21">
         <v>135</v>
@@ -12502,13 +12487,13 @@
         <v>315</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>990</v>
+        <v>982</v>
       </c>
       <c r="G17" s="22" t="s">
         <v>575</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I17" s="21">
         <v>135</v>
@@ -12527,13 +12512,13 @@
         <v>316</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>991</v>
+        <v>983</v>
       </c>
       <c r="G18" s="22" t="s">
         <v>573</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I18" s="21">
         <v>135</v>
@@ -12552,13 +12537,13 @@
         <v>317</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>988</v>
+        <v>980</v>
       </c>
       <c r="G19" s="22" t="s">
         <v>577</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I19" s="21">
         <v>135</v>
@@ -12578,7 +12563,7 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I20" s="1">
         <v>135</v>
@@ -12595,7 +12580,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I21" s="1">
         <v>135</v>
@@ -12614,7 +12599,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I22" s="1">
         <v>135</v>
@@ -12631,13 +12616,13 @@
         <v>689</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>886</v>
+        <v>878</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>578</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I23" s="1">
         <v>135</v>
@@ -12654,13 +12639,13 @@
         <v>325</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>887</v>
+        <v>879</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>892</v>
+        <v>884</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I24" s="1">
         <v>135</v>
@@ -12679,13 +12664,13 @@
         <v>326</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>888</v>
+        <v>880</v>
       </c>
       <c r="G25" s="15" t="s">
         <v>579</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I25" s="1">
         <v>135</v>
@@ -12704,13 +12689,13 @@
         <v>327</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>889</v>
+        <v>881</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>580</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I26" s="1">
         <v>135</v>
@@ -12729,13 +12714,13 @@
         <v>328</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>890</v>
+        <v>882</v>
       </c>
       <c r="G27" s="15" t="s">
         <v>581</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I27" s="1">
         <v>135</v>
@@ -12754,13 +12739,13 @@
         <v>329</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>891</v>
+        <v>883</v>
       </c>
       <c r="G28" s="15" t="s">
-        <v>893</v>
+        <v>885</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I28" s="1">
         <v>135</v>
@@ -12780,7 +12765,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I29" s="1">
         <v>135</v>
@@ -12797,7 +12782,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I30" s="1">
         <v>135</v>
@@ -12816,7 +12801,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I31" s="1">
         <v>135</v>
@@ -12841,7 +12826,7 @@
         <v>583</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I32" s="21">
         <v>135</v>
@@ -12866,7 +12851,7 @@
         <v>155</v>
       </c>
       <c r="H33" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I33" s="21">
         <v>135</v>
@@ -12891,7 +12876,7 @@
         <v>157</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I34" s="21">
         <v>135</v>
@@ -12912,7 +12897,7 @@
       <c r="F35" s="21"/>
       <c r="G35" s="21"/>
       <c r="H35" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I35" s="21">
         <v>135</v>
@@ -12937,7 +12922,7 @@
         <v>585</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I36" s="21">
         <v>135</v>
@@ -12961,7 +12946,7 @@
       <c r="F37" s="21"/>
       <c r="G37" s="21"/>
       <c r="H37" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I37" s="21">
         <v>135</v>
@@ -12982,7 +12967,7 @@
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
       <c r="H38" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I38" s="21">
         <v>135</v>
@@ -13003,7 +12988,7 @@
       <c r="F39" s="22"/>
       <c r="G39" s="22"/>
       <c r="H39" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I39" s="21">
         <v>135</v>
@@ -13024,7 +13009,7 @@
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
       <c r="H40" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I40" s="21">
         <v>135</v>
@@ -13045,7 +13030,7 @@
       <c r="F41" s="21"/>
       <c r="G41" s="21"/>
       <c r="H41" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I41" s="21">
         <v>135</v>
@@ -13066,7 +13051,7 @@
       <c r="F42" s="21"/>
       <c r="G42" s="21"/>
       <c r="H42" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I42" s="21">
         <v>135</v>
@@ -13091,7 +13076,7 @@
         <v>587</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I43" s="21">
         <v>135</v>
@@ -13112,7 +13097,7 @@
       <c r="F44" s="22"/>
       <c r="G44" s="22"/>
       <c r="H44" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I44" s="21">
         <v>135</v>
@@ -13137,7 +13122,7 @@
         <v>589</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I45" s="21">
         <v>135</v>
@@ -13158,7 +13143,7 @@
       <c r="F46" s="21"/>
       <c r="G46" s="21"/>
       <c r="H46" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I46" s="21">
         <v>135</v>
@@ -13179,7 +13164,7 @@
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
       <c r="H47" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I47" s="21">
         <v>135</v>
@@ -13200,7 +13185,7 @@
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
       <c r="H48" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I48" s="21">
         <v>135</v>
@@ -13221,7 +13206,7 @@
       <c r="F49" s="21"/>
       <c r="G49" s="21"/>
       <c r="H49" s="21" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I49" s="21">
         <v>135</v>
@@ -13242,7 +13227,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I50" s="1">
         <v>135</v>
@@ -13263,7 +13248,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I51" s="1">
         <v>135</v>
@@ -13284,7 +13269,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I52" s="1">
         <v>135</v>
@@ -13305,7 +13290,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I53" s="1">
         <v>135</v>
@@ -13330,7 +13315,7 @@
         <v>806</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I54" s="1">
         <v>135</v>
@@ -13353,7 +13338,7 @@
         <v>157</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I55" s="1">
         <v>135</v>
@@ -13376,7 +13361,7 @@
         <v>155</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I56" s="1">
         <v>135</v>
@@ -13401,7 +13386,7 @@
         <v>808</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I57" s="1">
         <v>135</v>
@@ -13420,13 +13405,13 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1" t="s">
-        <v>1006</v>
+        <v>998</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>1005</v>
+        <v>997</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I58" s="1">
         <v>135</v>
@@ -13449,7 +13434,7 @@
         <v>157</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I59" s="1">
         <v>135</v>
@@ -13472,7 +13457,7 @@
         <v>155</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I60" s="1">
         <v>135</v>
@@ -13497,7 +13482,7 @@
         <v>810</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I61" s="1">
         <v>135</v>
@@ -13520,7 +13505,7 @@
         <v>157</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I62" s="1">
         <v>135</v>
@@ -13543,7 +13528,7 @@
         <v>155</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I63" s="1">
         <v>135</v>
@@ -13562,7 +13547,7 @@
         <v>812</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I64" s="1">
         <v>135</v>
@@ -13583,7 +13568,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I65" s="1">
         <v>135</v>
@@ -13604,7 +13589,7 @@
       <c r="F66" s="10"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I66" s="1">
         <v>135</v>
@@ -13625,7 +13610,7 @@
       <c r="F67" s="10"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I67" s="1">
         <v>135</v>
@@ -13646,7 +13631,7 @@
       <c r="F68" s="10"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I68" s="1">
         <v>135</v>
@@ -13667,7 +13652,7 @@
       <c r="F69" s="10"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I69" s="1">
         <v>135</v>
@@ -13688,7 +13673,7 @@
       <c r="F70" s="10"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I70" s="1">
         <v>135</v>
@@ -13709,7 +13694,7 @@
       <c r="F71" s="10"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I71" s="1">
         <v>135</v>
@@ -13730,7 +13715,7 @@
       <c r="F72" s="10"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I72" s="1">
         <v>135</v>
@@ -13751,7 +13736,7 @@
       <c r="F73" s="10"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I73" s="1">
         <v>135</v>
@@ -13772,7 +13757,7 @@
       <c r="F74" s="10"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I74" s="1">
         <v>135</v>
@@ -13793,7 +13778,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I75" s="1">
         <v>135</v>
@@ -13812,13 +13797,13 @@
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1" t="s">
-        <v>1004</v>
+        <v>996</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>1003</v>
+        <v>995</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I76" s="1">
         <v>135</v>
@@ -13843,7 +13828,7 @@
         <v>814</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I77" s="1">
         <v>135</v>
@@ -13868,7 +13853,7 @@
         <v>816</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I78" s="1">
         <v>135</v>
@@ -13893,7 +13878,7 @@
         <v>818</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I79" s="1">
         <v>135</v>
@@ -13912,13 +13897,13 @@
         <v>714</v>
       </c>
       <c r="F80" s="41" t="s">
-        <v>993</v>
+        <v>985</v>
       </c>
       <c r="G80" s="41" t="s">
-        <v>994</v>
+        <v>986</v>
       </c>
       <c r="H80" s="40" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I80" s="40">
         <v>135</v>
@@ -13943,7 +13928,7 @@
         <v>820</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I81" s="1">
         <v>135</v>
@@ -13968,7 +13953,7 @@
         <v>822</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I82" s="1">
         <v>135</v>
@@ -13993,7 +13978,7 @@
         <v>824</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I83" s="1">
         <v>135</v>
@@ -14014,7 +13999,7 @@
       <c r="F84" s="9"/>
       <c r="G84" s="5"/>
       <c r="H84" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I84" s="1">
         <v>135</v>
@@ -14035,7 +14020,7 @@
       <c r="F85" s="9"/>
       <c r="G85" s="5"/>
       <c r="H85" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I85" s="1">
         <v>135</v>
@@ -14056,7 +14041,7 @@
       <c r="F86" s="9"/>
       <c r="G86" s="5"/>
       <c r="H86" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I86" s="1">
         <v>135</v>
@@ -14077,7 +14062,7 @@
       <c r="F87" s="9"/>
       <c r="G87" s="5"/>
       <c r="H87" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I87" s="1">
         <v>135</v>
@@ -14098,7 +14083,7 @@
       <c r="F88" s="9"/>
       <c r="G88" s="5"/>
       <c r="H88" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I88" s="1">
         <v>135</v>
@@ -14119,7 +14104,7 @@
       <c r="F89" s="9"/>
       <c r="G89" s="5"/>
       <c r="H89" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I89" s="1">
         <v>135</v>
@@ -14144,7 +14129,7 @@
         <v>836</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I90" s="1">
         <v>135</v>
@@ -14169,7 +14154,7 @@
         <v>826</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I91" s="1">
         <v>135</v>
@@ -14194,7 +14179,7 @@
         <v>828</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I92" s="1">
         <v>135</v>
@@ -14219,7 +14204,7 @@
         <v>830</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I93" s="1">
         <v>135</v>
@@ -14244,7 +14229,7 @@
         <v>832</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I94" s="1">
         <v>135</v>
@@ -14269,7 +14254,7 @@
         <v>834</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I95" s="1">
         <v>135</v>
@@ -14294,7 +14279,7 @@
         <v>838</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I96" s="1">
         <v>135</v>
@@ -14312,13 +14297,13 @@
       </c>
       <c r="E97" s="20"/>
       <c r="F97" s="20" t="s">
-        <v>931</v>
+        <v>923</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="H97" s="20" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I97" s="20">
         <v>135</v>
@@ -14337,13 +14322,13 @@
         <v>530</v>
       </c>
       <c r="F98" s="38" t="s">
-        <v>929</v>
+        <v>921</v>
       </c>
       <c r="G98" s="38" t="s">
-        <v>930</v>
+        <v>922</v>
       </c>
       <c r="H98" s="20" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I98" s="20">
         <v>135</v>
@@ -14362,13 +14347,13 @@
         <v>532</v>
       </c>
       <c r="F99" s="38" t="s">
-        <v>932</v>
+        <v>924</v>
       </c>
       <c r="G99" s="38" t="s">
-        <v>933</v>
+        <v>925</v>
       </c>
       <c r="H99" s="20" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I99" s="20">
         <v>135</v>
@@ -14387,13 +14372,13 @@
         <v>534</v>
       </c>
       <c r="F100" s="38" t="s">
-        <v>934</v>
+        <v>926</v>
       </c>
       <c r="G100" s="38" t="s">
-        <v>935</v>
+        <v>927</v>
       </c>
       <c r="H100" s="20" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I100" s="20">
         <v>135</v>
@@ -14412,13 +14397,13 @@
         <v>537</v>
       </c>
       <c r="F101" s="38" t="s">
-        <v>936</v>
+        <v>928</v>
       </c>
       <c r="G101" s="38" t="s">
-        <v>937</v>
+        <v>929</v>
       </c>
       <c r="H101" s="20" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I101" s="20">
         <v>135</v>
@@ -14437,13 +14422,13 @@
       <c r="D102" s="40"/>
       <c r="E102" s="40"/>
       <c r="F102" s="40" t="s">
-        <v>995</v>
+        <v>987</v>
       </c>
       <c r="G102" s="40" t="s">
-        <v>996</v>
+        <v>988</v>
       </c>
       <c r="H102" s="40" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I102" s="40">
         <v>135</v>
@@ -14462,13 +14447,13 @@
       <c r="D103" s="40"/>
       <c r="E103" s="40"/>
       <c r="F103" s="40" t="s">
-        <v>997</v>
+        <v>989</v>
       </c>
       <c r="G103" s="40" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="H103" s="40" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I103" s="40">
         <v>135</v>
@@ -14487,13 +14472,13 @@
       <c r="D104" s="43"/>
       <c r="E104" s="43"/>
       <c r="F104" s="45" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="G104" s="43" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="H104" s="43" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I104" s="43">
         <v>135</v>
@@ -14518,7 +14503,7 @@
         <v>840</v>
       </c>
       <c r="H105" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I105" s="14">
         <v>135</v>
@@ -14543,7 +14528,7 @@
         <v>842</v>
       </c>
       <c r="H106" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I106" s="14">
         <v>135</v>
@@ -14568,7 +14553,7 @@
         <v>844</v>
       </c>
       <c r="H107" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I107" s="14">
         <v>135</v>
@@ -14593,7 +14578,7 @@
         <v>846</v>
       </c>
       <c r="H108" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I108" s="14">
         <v>135</v>
@@ -14618,7 +14603,7 @@
         <v>848</v>
       </c>
       <c r="H109" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I109" s="14">
         <v>135</v>
@@ -14643,7 +14628,7 @@
         <v>850</v>
       </c>
       <c r="H110" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I110" s="14">
         <v>135</v>
@@ -14668,7 +14653,7 @@
         <v>661</v>
       </c>
       <c r="H111" s="20" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I111" s="20">
         <v>135</v>
@@ -14687,13 +14672,13 @@
       <c r="D112" s="40"/>
       <c r="E112" s="40"/>
       <c r="F112" s="40" t="s">
-        <v>998</v>
+        <v>990</v>
       </c>
       <c r="G112" s="40" t="s">
-        <v>999</v>
+        <v>991</v>
       </c>
       <c r="H112" s="40" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I112" s="40">
         <v>135</v>
@@ -14712,13 +14697,13 @@
       <c r="D113" s="40"/>
       <c r="E113" s="40"/>
       <c r="F113" s="40" t="s">
-        <v>1000</v>
+        <v>992</v>
       </c>
       <c r="G113" s="40" t="s">
-        <v>1001</v>
+        <v>993</v>
       </c>
       <c r="H113" s="40" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I113" s="40">
         <v>135</v>
@@ -14743,7 +14728,7 @@
         <v>666</v>
       </c>
       <c r="H114" s="40" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I114" s="40">
         <v>135</v>
@@ -14768,7 +14753,7 @@
         <v>848</v>
       </c>
       <c r="H115" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I115" s="14">
         <v>135</v>
@@ -14793,7 +14778,7 @@
         <v>852</v>
       </c>
       <c r="H116" s="14" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I116" s="14">
         <v>135</v>
@@ -14811,14 +14796,10 @@
       </c>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
-      <c r="F117" s="11" t="s">
-        <v>853</v>
-      </c>
-      <c r="G117" s="11" t="s">
-        <v>854</v>
-      </c>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
       <c r="H117" s="11" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I117" s="11">
         <v>135</v>
@@ -14837,13 +14818,13 @@
         <v>770</v>
       </c>
       <c r="F118" s="12" t="s">
-        <v>855</v>
+        <v>1000</v>
       </c>
       <c r="G118" s="12" t="s">
-        <v>856</v>
+        <v>1001</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I118" s="11">
         <v>135</v>
@@ -14862,13 +14843,13 @@
         <v>771</v>
       </c>
       <c r="F119" s="12" t="s">
-        <v>857</v>
+        <v>999</v>
       </c>
       <c r="G119" s="12" t="s">
-        <v>858</v>
+        <v>1001</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I119" s="11">
         <v>135</v>
@@ -14887,13 +14868,13 @@
         <v>772</v>
       </c>
       <c r="F120" s="12" t="s">
-        <v>859</v>
+        <v>774</v>
       </c>
       <c r="G120" s="12" t="s">
-        <v>860</v>
+        <v>1001</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I120" s="11">
         <v>135</v>
@@ -14912,13 +14893,13 @@
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1" t="s">
-        <v>861</v>
+        <v>853</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>862</v>
+        <v>854</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I121" s="1">
         <v>135</v>
@@ -14937,13 +14918,13 @@
         <v>779</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>863</v>
+        <v>855</v>
       </c>
       <c r="G122" s="5" t="s">
-        <v>864</v>
+        <v>856</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I122" s="1">
         <v>135</v>
@@ -14962,13 +14943,13 @@
         <v>780</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I123" s="1">
         <v>135</v>
@@ -14987,13 +14968,13 @@
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I124" s="1">
         <v>135</v>
@@ -15016,7 +14997,7 @@
         <v>157</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I125" s="1">
         <v>135</v>
@@ -15039,7 +15020,7 @@
         <v>155</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I126" s="1">
         <v>135</v>
@@ -15058,13 +15039,13 @@
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1" t="s">
-        <v>865</v>
+        <v>857</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>866</v>
+        <v>858</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I127" s="1">
         <v>135</v>
@@ -15083,13 +15064,13 @@
         <v>787</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>869</v>
+        <v>861</v>
       </c>
       <c r="G128" s="5" t="s">
-        <v>870</v>
+        <v>862</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I128" s="1">
         <v>135</v>
@@ -15108,13 +15089,13 @@
         <v>788</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>871</v>
+        <v>863</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>872</v>
+        <v>864</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I129" s="1">
         <v>135</v>
@@ -15133,13 +15114,13 @@
         <v>789</v>
       </c>
       <c r="F130" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="G130" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="H130" s="1" t="s">
         <v>873</v>
-      </c>
-      <c r="G130" s="5" t="s">
-        <v>874</v>
-      </c>
-      <c r="H130" s="1" t="s">
-        <v>881</v>
       </c>
       <c r="I130" s="1">
         <v>135</v>
@@ -15158,13 +15139,13 @@
         <v>790</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>875</v>
+        <v>867</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>876</v>
+        <v>868</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I131" s="1">
         <v>135</v>
@@ -15183,13 +15164,13 @@
         <v>791</v>
       </c>
       <c r="F132" s="5" t="s">
-        <v>877</v>
+        <v>869</v>
       </c>
       <c r="G132" s="5" t="s">
-        <v>878</v>
+        <v>870</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I132" s="1">
         <v>135</v>
@@ -15214,7 +15195,7 @@
         <v>850</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I133" s="1">
         <v>135</v>
@@ -15233,13 +15214,13 @@
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1" t="s">
-        <v>867</v>
+        <v>859</v>
       </c>
       <c r="G134" s="1" t="s">
-        <v>868</v>
+        <v>860</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I134" s="1">
         <v>135</v>
@@ -15262,7 +15243,7 @@
         <v>157</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I135" s="1">
         <v>135</v>
@@ -15285,7 +15266,7 @@
         <v>155</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I136" s="1">
         <v>135</v>
@@ -15304,13 +15285,13 @@
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1" t="s">
-        <v>879</v>
+        <v>871</v>
       </c>
       <c r="G137" s="1" t="s">
-        <v>880</v>
+        <v>872</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I137" s="1">
         <v>135</v>
@@ -15327,7 +15308,7 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I138" s="1">
         <v>135</v>
@@ -15344,7 +15325,7 @@
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I139" s="1">
         <v>135</v>
@@ -15361,7 +15342,7 @@
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I140" s="1">
         <v>135</v>
@@ -15378,7 +15359,7 @@
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I141" s="1">
         <v>135</v>
@@ -15395,7 +15376,7 @@
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I142" s="1">
         <v>135</v>
@@ -15412,7 +15393,7 @@
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I143" s="1">
         <v>135</v>
@@ -15429,7 +15410,7 @@
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I144" s="1">
         <v>135</v>
@@ -15446,7 +15427,7 @@
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I145" s="1">
         <v>135</v>
@@ -15463,7 +15444,7 @@
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I146" s="1">
         <v>135</v>
@@ -15480,7 +15461,7 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I147" s="1">
         <v>135</v>
@@ -15497,7 +15478,7 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I148" s="1">
         <v>135</v>
@@ -15514,7 +15495,7 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I149" s="1">
         <v>135</v>
@@ -15531,7 +15512,7 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I150" s="1">
         <v>135</v>
@@ -15548,7 +15529,7 @@
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I151" s="1">
         <v>135</v>
@@ -15565,7 +15546,7 @@
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I152" s="1">
         <v>135</v>
@@ -15582,7 +15563,7 @@
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I153" s="1">
         <v>135</v>
@@ -15599,7 +15580,7 @@
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I154" s="1">
         <v>135</v>
@@ -15616,7 +15597,7 @@
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I155" s="1">
         <v>135</v>
@@ -15633,7 +15614,7 @@
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
       <c r="H156" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I156" s="1">
         <v>135</v>
@@ -15650,7 +15631,7 @@
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I157" s="1">
         <v>135</v>
@@ -15667,7 +15648,7 @@
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I158" s="1">
         <v>135</v>
@@ -15684,7 +15665,7 @@
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1" t="s">
-        <v>881</v>
+        <v>873</v>
       </c>
       <c r="I159" s="1">
         <v>135</v>
@@ -15722,42 +15703,42 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.45">
       <c r="A1" s="24" t="s">
-        <v>896</v>
+        <v>888</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>897</v>
+        <v>889</v>
       </c>
       <c r="C1" s="25" t="s">
-        <v>898</v>
+        <v>890</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>899</v>
+        <v>891</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>900</v>
+        <v>892</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>901</v>
+        <v>893</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>902</v>
+        <v>894</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.45">
       <c r="A2" s="26" t="s">
-        <v>903</v>
+        <v>895</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>904</v>
+        <v>896</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>906</v>
+        <v>898</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>907</v>
+        <v>899</v>
       </c>
       <c r="F2" s="29">
         <v>1480</v>
@@ -15768,13 +15749,13 @@
     </row>
     <row r="3" spans="1:7" ht="15.45">
       <c r="A3" s="26" t="s">
-        <v>908</v>
+        <v>900</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
@@ -15783,19 +15764,19 @@
     </row>
     <row r="4" spans="1:7" ht="15.45">
       <c r="A4" s="31" t="s">
-        <v>910</v>
+        <v>902</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="C4" s="33" t="s">
+        <v>897</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>904</v>
+      </c>
+      <c r="E4" s="33" t="s">
         <v>905</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>912</v>
-      </c>
-      <c r="E4" s="33" t="s">
-        <v>913</v>
       </c>
       <c r="F4" s="34">
         <v>5497</v>
@@ -15806,16 +15787,16 @@
     </row>
     <row r="5" spans="1:7" ht="15.45">
       <c r="A5" s="31" t="s">
-        <v>914</v>
+        <v>906</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>915</v>
+        <v>907</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>916</v>
+        <v>908</v>
       </c>
       <c r="E5" s="35"/>
       <c r="F5" s="35"/>
@@ -15823,13 +15804,13 @@
     </row>
     <row r="6" spans="1:7" ht="15.45">
       <c r="A6" s="31" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="35"/>
@@ -15838,19 +15819,19 @@
     </row>
     <row r="7" spans="1:7" ht="15.45">
       <c r="A7" s="31" t="s">
-        <v>919</v>
+        <v>911</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>911</v>
+        <v>903</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>920</v>
+        <v>912</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>921</v>
+        <v>913</v>
       </c>
       <c r="F7" s="34">
         <v>856</v>
@@ -15861,16 +15842,16 @@
     </row>
     <row r="8" spans="1:7" ht="15.45">
       <c r="A8" s="31" t="s">
-        <v>922</v>
+        <v>914</v>
       </c>
       <c r="B8" s="35" t="s">
+        <v>907</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>897</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>915</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>905</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>923</v>
       </c>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
@@ -15878,13 +15859,13 @@
     </row>
     <row r="9" spans="1:7" ht="15.45">
       <c r="A9" s="31" t="s">
-        <v>917</v>
+        <v>909</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>918</v>
+        <v>910</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D9" s="35"/>
       <c r="E9" s="35"/>
@@ -15893,19 +15874,19 @@
     </row>
     <row r="10" spans="1:7" ht="15.45">
       <c r="A10" s="31" t="s">
-        <v>924</v>
+        <v>916</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>925</v>
+        <v>917</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>926</v>
+        <v>918</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>927</v>
+        <v>919</v>
       </c>
       <c r="F10" s="36">
         <v>1607</v>
@@ -15916,13 +15897,13 @@
     </row>
     <row r="11" spans="1:7" ht="15.45">
       <c r="A11" s="31" t="s">
-        <v>928</v>
+        <v>920</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>909</v>
+        <v>901</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>905</v>
+        <v>897</v>
       </c>
       <c r="D11" s="35"/>
       <c r="E11" s="35"/>

</xml_diff>

<commit_message>
Add ENROLLMENT DATE in SECTION 1 as Date of Linked to Treatment
</commit_message>
<xml_diff>
--- a/rhies_OpenMRStoDHIS2Mediator/matchingDico/DHIS2DataElementToOpenMRS.xlsx
+++ b/rhies_OpenMRStoDHIS2Mediator/matchingDico/DHIS2DataElementToOpenMRS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SavicsProject\RHIES\RHIESMediators\coding\rhies_Mediators\rhies_OpenMRStoDHIS2Mediator\matchingDico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F40522-EEA5-46F6-84E3-706B93CD655D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF34E5E5-8308-470C-B63C-282CAB347749}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="r45yv7rwDEO" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1855" uniqueCount="1002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="1004">
   <si>
     <t>DHIS2 dropdown name</t>
   </si>
@@ -3088,6 +3088,12 @@
   </si>
   <si>
     <t>Text</t>
+  </si>
+  <si>
+    <t>badacf97-0970-4dde-aee4-5e1c2bb125f7</t>
+  </si>
+  <si>
+    <t>ENROLLMENT DATE</t>
   </si>
 </sst>
 </file>
@@ -7822,8 +7828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F78C531-5A28-448B-9C94-8E675119435D}">
   <dimension ref="A1:J191"/>
   <sheetViews>
-    <sheetView showFormulas="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B101" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="58.921875" defaultRowHeight="14.6"/>
@@ -10962,8 +10968,12 @@
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
-      <c r="F135" s="1"/>
-      <c r="G135" s="1"/>
+      <c r="F135" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="G135" s="1" t="s">
+        <v>1002</v>
+      </c>
       <c r="H135" s="1" t="s">
         <v>556</v>
       </c>
@@ -12103,12 +12113,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DC28AE1-BBA6-488B-8021-D9435874BC68}">
   <dimension ref="A1:J159"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B125" activePane="bottomRight" state="frozen"/>
       <selection activeCell="K8" sqref="K8"/>
       <selection pane="topRight" activeCell="K8" sqref="K8"/>
       <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
-      <selection pane="bottomRight" activeCell="F121" sqref="F121"/>
+      <selection pane="bottomRight" activeCell="F99" sqref="F99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="64.61328125" defaultRowHeight="14.6"/>

</xml_diff>